<commit_message>
refactoring applicant and officer
</commit_message>
<xml_diff>
--- a/data/InquiryList.xlsx
+++ b/data/InquiryList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ApplicantNRIC</t>
   </si>
@@ -27,6 +27,15 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t>S1234567A</t>
+  </si>
+  <si>
+    <t>fuck</t>
+  </si>
+  <si>
+    <t>Acacia Breeze</t>
   </si>
 </sst>
 </file>
@@ -74,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -97,6 +106,21 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" t="n" s="1">
+        <v>45767.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>